<commit_message>
Spreadsheet as used to derive keymap.c for branch
</commit_message>
<xml_diff>
--- a/IRST-Preonic.xlsx
+++ b/IRST-Preonic.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/21726f12972b465d/Documents/IRST layout/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VC\git\QMK-wips\ISRT_Preonic_QMK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD1A8A77-4B87-4279-A312-EE41A807DC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D301511-849E-42D3-9EAB-267CB7B42489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{7F5A7B0C-20EC-4E02-B09B-1C5B3AC45F48}"/>
   </bookViews>
@@ -111,24 +111,12 @@
     <t>KC_S</t>
   </si>
   <si>
-    <t>MT(MOD_LALT,KC_R)</t>
-  </si>
-  <si>
-    <t>MT(MOD_LGUI,KC_T)</t>
-  </si>
-  <si>
     <t>KC_G</t>
   </si>
   <si>
     <t>KC_P</t>
   </si>
   <si>
-    <t>MT(MOD_RGUI,KC_N)</t>
-  </si>
-  <si>
-    <t>MT(MOD_RALT,KC_E)</t>
-  </si>
-  <si>
     <t>KC_A</t>
   </si>
   <si>
@@ -496,6 +484,18 @@
   </si>
   <si>
     <t>KC_NO</t>
+  </si>
+  <si>
+    <t>KC_R</t>
+  </si>
+  <si>
+    <t>KC_T</t>
+  </si>
+  <si>
+    <t>KC_N</t>
+  </si>
+  <si>
+    <t>KC_E</t>
   </si>
 </sst>
 </file>
@@ -815,28 +815,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA8E771A-6ED3-4E26-8B8E-3539F8660439}" name="Layout_0" displayName="Layout_0" comment="layer for typing alphabetic keys, (l.c. &amp; u.c.) some modifiers and layer chosers" ref="A2:L7" totalsRowShown="0" tableBorderDxfId="7">
-  <autoFilter ref="A2:L7" xr:uid="{DA8E771A-6ED3-4E26-8B8E-3539F8660439}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{06F0293D-7D3D-4A04-952C-9924613F0CA1}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{D15FE5C6-BE24-4C5F-BF3D-800BD84B3969}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{D267651C-D719-44CF-B219-AC4186FF423C}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{0F16A937-6C00-480A-B12B-BE9267E94D39}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{55AAC62B-ADF9-40AB-8A4F-5F7EBD916384}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{0F581A58-67E2-4C70-94DB-0DCA34D367BD}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{D0CC4A30-6DA4-4536-853E-1C85C009027A}" name="Column7" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{486753A8-F426-4C12-B6B1-496C654F5E85}" name="Column8"/>
-    <tableColumn id="9" xr3:uid="{A7B33429-9866-4807-97A9-D9207BCA1075}" name="Column9"/>
-    <tableColumn id="10" xr3:uid="{CBCF11CC-F7FC-4C8F-BAEC-FF4B5ECF7495}" name="Column10"/>
-    <tableColumn id="11" xr3:uid="{AD352A13-B624-4B23-AE14-9C355E0205F3}" name="Column11"/>
-    <tableColumn id="12" xr3:uid="{7710C233-8F5D-44FD-8DC7-4B0C41A6F3A7}" name="Column12"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{511E6A67-7E1A-47C0-8151-E1E6E95AE019}" name="Layout_1" displayName="Layout_1" ref="A10:L15" totalsRowShown="0" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{511E6A67-7E1A-47C0-8151-E1E6E95AE019}" name="Layout_1" displayName="Layout_1" ref="A10:L15" totalsRowShown="0" tableBorderDxfId="7">
   <autoFilter ref="A10:L15" xr:uid="{511E6A67-7E1A-47C0-8151-E1E6E95AE019}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{73CB4919-8AD2-47E5-9CD9-0A336BF728B6}" name="Column1"/>
@@ -845,7 +824,7 @@
     <tableColumn id="4" xr3:uid="{5828FBFA-3630-442F-B460-0E1895E7A172}" name="Column4"/>
     <tableColumn id="5" xr3:uid="{AE5CC2F3-E347-43BA-AB86-536E5242FABD}" name="Column5"/>
     <tableColumn id="6" xr3:uid="{74FDAE23-8A99-4496-8722-8E9271682D31}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{D92D7203-F474-4B1C-8E26-1AC66664C964}" name="Column7" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{D92D7203-F474-4B1C-8E26-1AC66664C964}" name="Column7" dataDxfId="6"/>
     <tableColumn id="8" xr3:uid="{A49D2154-9786-42FC-8E9B-CC3FD0A2087C}" name="Column8"/>
     <tableColumn id="9" xr3:uid="{CB8A3735-B5A1-460A-9ACD-F08411D7509B}" name="Column9"/>
     <tableColumn id="10" xr3:uid="{6C10E492-B6CB-46C1-86BA-4261E4BD85C6}" name="Column10"/>
@@ -856,8 +835,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F03AAAB4-4A68-4AD7-8707-F301F6CC0E21}" name="Layout_2" displayName="Layout_2" ref="A18:L24" totalsRowShown="0" tableBorderDxfId="3">
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F03AAAB4-4A68-4AD7-8707-F301F6CC0E21}" name="Layout_2" displayName="Layout_2" ref="A18:L24" totalsRowShown="0" tableBorderDxfId="5">
   <autoFilter ref="A18:L24" xr:uid="{F03AAAB4-4A68-4AD7-8707-F301F6CC0E21}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{426078B5-3024-4110-B87E-031A4EBB1B67}" name="Column1"/>
@@ -866,7 +845,7 @@
     <tableColumn id="4" xr3:uid="{AADED880-005E-4D9E-A688-B384286A3678}" name="Column4"/>
     <tableColumn id="5" xr3:uid="{77571823-C872-46A2-87A3-308D87A006C2}" name="Column5"/>
     <tableColumn id="6" xr3:uid="{972D301F-915B-44B0-ACB0-F91680518982}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{B33835EE-4BCB-4BDD-80D9-13BC6133BE2C}" name="Column7" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{B33835EE-4BCB-4BDD-80D9-13BC6133BE2C}" name="Column7" dataDxfId="4"/>
     <tableColumn id="8" xr3:uid="{094E239B-B60A-4C08-9320-F5ACB77B7C5C}" name="Column8"/>
     <tableColumn id="9" xr3:uid="{6C32C8AA-1C32-4DB6-A2DD-AD7541EED119}" name="Column9"/>
     <tableColumn id="10" xr3:uid="{A5550E70-D31E-4A02-86E1-05260A5F9323}" name="Column10"/>
@@ -877,8 +856,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4D718204-1D23-4F24-B0F0-D99F73CC9698}" name="Layout_3" displayName="Layout_3" ref="A26:L31" totalsRowShown="0" tableBorderDxfId="1">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4D718204-1D23-4F24-B0F0-D99F73CC9698}" name="Layout_3" displayName="Layout_3" ref="A26:L31" totalsRowShown="0" tableBorderDxfId="3">
   <autoFilter ref="A26:L31" xr:uid="{4D718204-1D23-4F24-B0F0-D99F73CC9698}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{99634A3A-068C-4A75-8F9F-6C0D8652E684}" name="Column1"/>
@@ -887,12 +866,33 @@
     <tableColumn id="4" xr3:uid="{88E14274-249F-409B-8C85-1A143CBC0A67}" name="Column4"/>
     <tableColumn id="5" xr3:uid="{9D63AEB0-6A69-4283-A2E6-65748C41AA23}" name="Column5"/>
     <tableColumn id="6" xr3:uid="{6727C674-62D7-4231-BF3F-95085E124D9B}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{684BFF8D-CCB6-4A20-A1A4-523035137815}" name="Column7" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{684BFF8D-CCB6-4A20-A1A4-523035137815}" name="Column7" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{68BCF398-9DC5-4A01-8DA3-E3CA729B3D24}" name="Column8"/>
     <tableColumn id="9" xr3:uid="{874F9AB6-4CE6-44C5-B4A8-8624455DED04}" name="Column9"/>
     <tableColumn id="10" xr3:uid="{D1958FF8-38AE-4363-8CC0-5930EE114F24}" name="Column10"/>
     <tableColumn id="11" xr3:uid="{A2C3F7A4-BF1C-49E6-99F8-5626744AC4B1}" name="Column11"/>
     <tableColumn id="12" xr3:uid="{2F714D4B-5876-46CA-8F39-92846B2D5474}" name="Column12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DF1341D6-9FD6-46BA-90E2-A2187C59ED4D}" name="Layout_03" displayName="Layout_03" comment="layer for typing alphabetic keys, (l.c. &amp; u.c.) some modifiers and layer chosers" ref="A2:L7" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A2:L7" xr:uid="{DF1341D6-9FD6-46BA-90E2-A2187C59ED4D}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{3855C516-71DC-4A31-9A26-5FDC79741CDE}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{DB93FBC9-282F-4650-AE14-ADE228DB1E75}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{84E08558-6A29-4D55-A530-28BE7FCD44C3}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{7F85DCE4-E8D6-4208-9917-59EEA26BD88E}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{016FE238-95E8-438C-AC70-9D513888593D}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{884264DD-782E-4781-A95C-809809F9314D}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{8887208C-3F86-4E10-958C-B95ABBAE24B9}" name="Column7" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{9610ABF7-5E86-4B4A-B20F-C863A16D0F9A}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{98BA5F9A-82E2-495A-8401-A8A16767A0FF}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{24595290-4C99-4254-8C8A-A986472C0DBA}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{C4CB28CA-30EA-45F8-8864-6E8B8D671A5F}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{16F34678-5E06-4EA3-9673-14E6F39F739F}" name="Column12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1198,7 +1198,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1277,37 +1277,37 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>50</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>51</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="K3" t="s">
         <v>53</v>
-      </c>
-      <c r="H3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" t="s">
-        <v>57</v>
       </c>
       <c r="L3" t="s">
         <v>22</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>13</v>
@@ -1348,12 +1348,12 @@
         <v>22</v>
       </c>
       <c r="L4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>23</v>
@@ -1362,107 +1362,107 @@
         <v>24</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="G5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="H5" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="K5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="L5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="G6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="H6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="I6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="J6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="K6" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>42</v>
-      </c>
       <c r="L6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" t="s">
         <v>64</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" t="s">
-        <v>66</v>
-      </c>
-      <c r="K7" t="s">
-        <v>67</v>
-      </c>
-      <c r="L7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1470,10 +1470,10 @@
     </row>
     <row r="9" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1526,192 +1526,192 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" t="s">
         <v>69</v>
       </c>
-      <c r="C12" t="s">
+      <c r="G12" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D12" t="s">
+      <c r="H12" t="s">
         <v>71</v>
       </c>
-      <c r="E12" t="s">
+      <c r="I12" t="s">
         <v>72</v>
       </c>
-      <c r="F12" t="s">
+      <c r="J12" t="s">
         <v>73</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" t="s">
-        <v>77</v>
       </c>
       <c r="K12" t="s">
         <v>22</v>
       </c>
       <c r="L12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" t="s">
         <v>78</v>
       </c>
-      <c r="C13" t="s">
+      <c r="G13" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D13" t="s">
+      <c r="H13" t="s">
         <v>80</v>
       </c>
-      <c r="E13" t="s">
+      <c r="I13" t="s">
         <v>81</v>
       </c>
-      <c r="F13" t="s">
+      <c r="J13" t="s">
         <v>82</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="K13" t="s">
         <v>83</v>
       </c>
-      <c r="H13" t="s">
-        <v>84</v>
-      </c>
-      <c r="I13" t="s">
-        <v>85</v>
-      </c>
-      <c r="J13" t="s">
-        <v>86</v>
-      </c>
-      <c r="K13" t="s">
-        <v>87</v>
-      </c>
       <c r="L13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" t="s">
         <v>88</v>
       </c>
-      <c r="C14" t="s">
+      <c r="G14" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D14" t="s">
+      <c r="H14" t="s">
         <v>90</v>
       </c>
-      <c r="E14" t="s">
+      <c r="I14" t="s">
         <v>91</v>
       </c>
-      <c r="F14" t="s">
+      <c r="J14" t="s">
         <v>92</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="K14" t="s">
         <v>93</v>
       </c>
-      <c r="H14" t="s">
-        <v>94</v>
-      </c>
-      <c r="I14" t="s">
-        <v>95</v>
-      </c>
-      <c r="J14" t="s">
-        <v>96</v>
-      </c>
-      <c r="K14" t="s">
-        <v>97</v>
-      </c>
       <c r="L14" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1719,10 +1719,10 @@
     </row>
     <row r="17" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1775,192 +1775,192 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D20" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>108</v>
-      </c>
       <c r="H20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I20" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E21" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I21" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="K21" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="L21" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" t="s">
         <v>113</v>
       </c>
-      <c r="C22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" t="s">
-        <v>117</v>
-      </c>
       <c r="G22" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C23" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D23" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E23" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H23" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I23" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J23" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K23" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L23" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1968,10 +1968,10 @@
     </row>
     <row r="25" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -2024,192 +2024,192 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" t="s">
         <v>119</v>
       </c>
-      <c r="C28" t="s">
+      <c r="G28" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D28" t="s">
+      <c r="H28" t="s">
         <v>121</v>
       </c>
-      <c r="E28" t="s">
+      <c r="I28" t="s">
         <v>122</v>
       </c>
-      <c r="F28" t="s">
+      <c r="J28" t="s">
         <v>123</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H28" t="s">
-        <v>125</v>
-      </c>
-      <c r="I28" t="s">
-        <v>126</v>
-      </c>
-      <c r="J28" t="s">
-        <v>127</v>
-      </c>
       <c r="K28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" t="s">
         <v>128</v>
       </c>
-      <c r="C29" t="s">
+      <c r="G29" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D29" t="s">
+      <c r="H29" t="s">
         <v>130</v>
       </c>
-      <c r="E29" t="s">
+      <c r="I29" t="s">
         <v>131</v>
       </c>
-      <c r="F29" t="s">
+      <c r="J29" t="s">
         <v>132</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="K29" t="s">
         <v>133</v>
       </c>
-      <c r="H29" t="s">
-        <v>134</v>
-      </c>
-      <c r="I29" t="s">
-        <v>135</v>
-      </c>
-      <c r="J29" t="s">
-        <v>136</v>
-      </c>
-      <c r="K29" t="s">
-        <v>137</v>
-      </c>
       <c r="L29" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C30" t="s">
+      <c r="H30" t="s">
         <v>139</v>
       </c>
-      <c r="D30" t="s">
+      <c r="I30" t="s">
         <v>140</v>
       </c>
-      <c r="E30" t="s">
+      <c r="J30" t="s">
         <v>141</v>
       </c>
-      <c r="F30" t="s">
-        <v>151</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="H30" t="s">
-        <v>143</v>
-      </c>
-      <c r="I30" t="s">
-        <v>144</v>
-      </c>
-      <c r="J30" t="s">
-        <v>145</v>
-      </c>
       <c r="K30" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="L30" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H31" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>